<commit_message>
🌟 init frontend de base base base tout à faire
</commit_message>
<xml_diff>
--- a/resources/Peuplement.xlsx
+++ b/resources/Peuplement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austin\CodeProjects\LivinParis\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliot\CodeProjects\LivInParis\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE3000-C02F-46AD-A962-FB2311D4F43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197C5CC-F447-4F8E-B922-1A6945DBDC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="16596" windowHeight="16656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="367">
   <si>
     <t>name</t>
   </si>
@@ -122,303 +122,153 @@
     <t>password</t>
   </si>
   <si>
-    <t>user0@example.com</t>
-  </si>
-  <si>
     <t>s)I7fTPUQk</t>
   </si>
   <si>
-    <t>user1@example.com</t>
-  </si>
-  <si>
     <t>4fSVDBi!!0</t>
   </si>
   <si>
-    <t>user2@example.com</t>
-  </si>
-  <si>
     <t>$2zwR0Ax%4</t>
   </si>
   <si>
-    <t>user3@example.com</t>
-  </si>
-  <si>
     <t>TRjUb@tw!8</t>
   </si>
   <si>
-    <t>user4@example.com</t>
-  </si>
-  <si>
     <t>#oK&amp;ozmqo0</t>
   </si>
   <si>
-    <t>user5@example.com</t>
-  </si>
-  <si>
     <t>+Ae$7ROe(w</t>
   </si>
   <si>
-    <t>user6@example.com</t>
-  </si>
-  <si>
     <t>oZ1gYQtxb$</t>
   </si>
   <si>
-    <t>user7@example.com</t>
-  </si>
-  <si>
     <t>)8jvgBhrod</t>
   </si>
   <si>
-    <t>user8@example.com</t>
-  </si>
-  <si>
     <t>)&amp;khBXtG7u</t>
   </si>
   <si>
-    <t>user9@example.com</t>
-  </si>
-  <si>
     <t>^^9ZrdnzWg</t>
   </si>
   <si>
-    <t>user10@example.com</t>
-  </si>
-  <si>
     <t>un+5jYd0_S</t>
   </si>
   <si>
-    <t>user11@example.com</t>
-  </si>
-  <si>
     <t>npzO4HsxM$</t>
   </si>
   <si>
-    <t>user12@example.com</t>
-  </si>
-  <si>
     <t>7A3v!vNk)Z</t>
   </si>
   <si>
-    <t>user13@example.com</t>
-  </si>
-  <si>
     <t>#kIXiDzwo3</t>
   </si>
   <si>
-    <t>user14@example.com</t>
-  </si>
-  <si>
     <t>)haVw0K5Y0</t>
   </si>
   <si>
-    <t>user15@example.com</t>
-  </si>
-  <si>
     <t>*+M$vHws87</t>
   </si>
   <si>
-    <t>user16@example.com</t>
-  </si>
-  <si>
     <t>eS1iY45t_C</t>
   </si>
   <si>
-    <t>user17@example.com</t>
-  </si>
-  <si>
     <t>5*80_CqKEs</t>
   </si>
   <si>
-    <t>user18@example.com</t>
-  </si>
-  <si>
     <t>C)7HlyPkLE</t>
   </si>
   <si>
-    <t>user19@example.com</t>
-  </si>
-  <si>
     <t>!uYT1koj0q</t>
   </si>
   <si>
-    <t>user20@example.com</t>
-  </si>
-  <si>
     <t>3REfJ1xf)l</t>
   </si>
   <si>
-    <t>user21@example.com</t>
-  </si>
-  <si>
     <t>&amp;)r4Cry^u8</t>
   </si>
   <si>
-    <t>user22@example.com</t>
-  </si>
-  <si>
     <t>+ah@IJvrY0</t>
   </si>
   <si>
-    <t>user23@example.com</t>
-  </si>
-  <si>
     <t>GV35Zs^@k+</t>
   </si>
   <si>
-    <t>user24@example.com</t>
-  </si>
-  <si>
     <t>BZfV4#3mk)</t>
   </si>
   <si>
-    <t>user25@example.com</t>
-  </si>
-  <si>
     <t>s9rY^GNj^*</t>
   </si>
   <si>
-    <t>user26@example.com</t>
-  </si>
-  <si>
     <t>$YlPRMFmm6</t>
   </si>
   <si>
-    <t>user27@example.com</t>
-  </si>
-  <si>
     <t>7R14LdWDs#</t>
   </si>
   <si>
-    <t>user28@example.com</t>
-  </si>
-  <si>
     <t>zHFumA_M_0</t>
   </si>
   <si>
-    <t>user29@example.com</t>
-  </si>
-  <si>
     <t>Y_65AYcmAw</t>
   </si>
   <si>
-    <t>user30@example.com</t>
-  </si>
-  <si>
     <t>3*1Ip3r9$)</t>
   </si>
   <si>
-    <t>user31@example.com</t>
-  </si>
-  <si>
     <t>p7C9(ZhfC+</t>
   </si>
   <si>
-    <t>user32@example.com</t>
-  </si>
-  <si>
     <t>E0QXke33!p</t>
   </si>
   <si>
-    <t>user33@example.com</t>
-  </si>
-  <si>
     <t>&amp;5TZlVT5#+</t>
   </si>
   <si>
-    <t>user34@example.com</t>
-  </si>
-  <si>
     <t>14tUIiXg%f</t>
   </si>
   <si>
-    <t>user35@example.com</t>
-  </si>
-  <si>
     <t>NN@3ZOe0oB</t>
   </si>
   <si>
-    <t>user36@example.com</t>
-  </si>
-  <si>
     <t>t*)0RRkvM5</t>
   </si>
   <si>
-    <t>user37@example.com</t>
-  </si>
-  <si>
     <t>XofrG5Yel+</t>
   </si>
   <si>
-    <t>user38@example.com</t>
-  </si>
-  <si>
     <t>UIdq(T1yO_</t>
   </si>
   <si>
-    <t>user39@example.com</t>
-  </si>
-  <si>
     <t>m0JLTVdx*6</t>
   </si>
   <si>
-    <t>user40@example.com</t>
-  </si>
-  <si>
     <t>2I1ZxCMh*3</t>
   </si>
   <si>
-    <t>user41@example.com</t>
-  </si>
-  <si>
     <t>$*+8r0Gilc</t>
   </si>
   <si>
-    <t>user42@example.com</t>
-  </si>
-  <si>
     <t>ju2aBjZ3)A</t>
   </si>
   <si>
-    <t>user43@example.com</t>
-  </si>
-  <si>
     <t>Uxk4CEss_f</t>
   </si>
   <si>
-    <t>user44@example.com</t>
-  </si>
-  <si>
     <t>Ce$*8FKiOV</t>
   </si>
   <si>
-    <t>user45@example.com</t>
-  </si>
-  <si>
     <t>(71^HTkiK%</t>
   </si>
   <si>
-    <t>user46@example.com</t>
-  </si>
-  <si>
     <t>#8QtYePQvs</t>
   </si>
   <si>
-    <t>user47@example.com</t>
-  </si>
-  <si>
     <t>e)d1wMWaH5</t>
   </si>
   <si>
-    <t>user48@example.com</t>
-  </si>
-  <si>
     <t>$CoANlwfV8</t>
   </si>
   <si>
-    <t>user49@example.com</t>
-  </si>
-  <si>
     <t>&amp;urSYkBR20</t>
   </si>
   <si>
@@ -1146,6 +996,159 @@
   </si>
   <si>
     <t>chef_is_banned</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>user0</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>user17</t>
+  </si>
+  <si>
+    <t>user18</t>
+  </si>
+  <si>
+    <t>user19</t>
+  </si>
+  <si>
+    <t>user20</t>
+  </si>
+  <si>
+    <t>user21</t>
+  </si>
+  <si>
+    <t>user22</t>
+  </si>
+  <si>
+    <t>user23</t>
+  </si>
+  <si>
+    <t>user24</t>
+  </si>
+  <si>
+    <t>user25</t>
+  </si>
+  <si>
+    <t>user26</t>
+  </si>
+  <si>
+    <t>user27</t>
+  </si>
+  <si>
+    <t>user28</t>
+  </si>
+  <si>
+    <t>user29</t>
+  </si>
+  <si>
+    <t>user30</t>
+  </si>
+  <si>
+    <t>user31</t>
+  </si>
+  <si>
+    <t>user32</t>
+  </si>
+  <si>
+    <t>user33</t>
+  </si>
+  <si>
+    <t>user34</t>
+  </si>
+  <si>
+    <t>user35</t>
+  </si>
+  <si>
+    <t>user36</t>
+  </si>
+  <si>
+    <t>user37</t>
+  </si>
+  <si>
+    <t>user38</t>
+  </si>
+  <si>
+    <t>user39</t>
+  </si>
+  <si>
+    <t>user40</t>
+  </si>
+  <si>
+    <t>user41</t>
+  </si>
+  <si>
+    <t>user42</t>
+  </si>
+  <si>
+    <t>user43</t>
+  </si>
+  <si>
+    <t>user44</t>
+  </si>
+  <si>
+    <t>user45</t>
+  </si>
+  <si>
+    <t>user46</t>
+  </si>
+  <si>
+    <t>user47</t>
+  </si>
+  <si>
+    <t>user48</t>
+  </si>
+  <si>
+    <t>user49</t>
   </si>
 </sst>
 </file>
@@ -1692,10 +1695,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1703,7 +1706,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1711,7 +1714,7 @@
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1719,7 +1722,7 @@
         <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1727,7 +1730,7 @@
         <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1735,7 +1738,7 @@
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1743,7 +1746,7 @@
         <v>937</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1751,7 +1754,7 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1759,7 +1762,7 @@
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1767,7 +1770,7 @@
         <v>568</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1775,7 +1778,7 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1783,7 +1786,7 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1791,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1799,7 +1802,7 @@
         <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1807,7 +1810,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1815,7 +1818,7 @@
         <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1823,7 +1826,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +1834,7 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1839,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +1850,7 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +1858,7 @@
         <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +1866,7 @@
         <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,7 +1874,7 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1879,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1887,7 +1890,7 @@
         <v>195</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1895,7 +1898,7 @@
         <v>979</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1903,7 +1906,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1911,7 +1914,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,7 +1922,7 @@
         <v>300</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1927,7 +1930,7 @@
         <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1935,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1943,7 +1946,7 @@
         <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1951,7 +1954,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1959,7 +1962,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,7 +1970,7 @@
         <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1975,7 +1978,7 @@
         <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1983,7 +1986,7 @@
         <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1991,7 +1994,7 @@
         <v>895</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1999,7 +2002,7 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2007,7 +2010,7 @@
         <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2015,7 +2018,7 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2023,7 +2026,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2031,7 +2034,7 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2039,7 +2042,7 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2047,7 +2050,7 @@
         <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2055,7 +2058,7 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2063,7 +2066,7 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2071,7 +2074,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2079,7 +2082,7 @@
         <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2087,7 +2090,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2095,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2116,13 +2119,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3212,19 +3215,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
       <c r="E1" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3232,7 +3235,7 @@
         <v>45768.203379629631</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -3249,7 +3252,7 @@
         <v>45769.850636574076</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -3266,7 +3269,7 @@
         <v>45772.54005787037</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C4">
         <v>13</v>
@@ -3283,7 +3286,7 @@
         <v>45772.506724537037</v>
       </c>
       <c r="B5" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -3300,7 +3303,7 @@
         <v>45772.591446759259</v>
       </c>
       <c r="B6" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3317,7 +3320,7 @@
         <v>45774.58965277778</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -3334,7 +3337,7 @@
         <v>45770.788032407407</v>
       </c>
       <c r="B8" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -3351,7 +3354,7 @@
         <v>45768.770509259259</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -3368,7 +3371,7 @@
         <v>45768.723981481482</v>
       </c>
       <c r="B10" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C10">
         <v>23</v>
@@ -3385,7 +3388,7 @@
         <v>45768.808703703704</v>
       </c>
       <c r="B11" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -3402,7 +3405,7 @@
         <v>45770.187256944446</v>
       </c>
       <c r="B12" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C12">
         <v>17</v>
@@ -3419,7 +3422,7 @@
         <v>45770.256701388891</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -3436,7 +3439,7 @@
         <v>45776.542314814818</v>
       </c>
       <c r="B14" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -3453,7 +3456,7 @@
         <v>45776.57912037037</v>
       </c>
       <c r="B15" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -3470,7 +3473,7 @@
         <v>45776.558287037034</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3487,7 +3490,7 @@
         <v>45771.94195601852</v>
       </c>
       <c r="B17" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C17">
         <v>19</v>
@@ -3504,7 +3507,7 @@
         <v>45771.976678240739</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -3521,7 +3524,7 @@
         <v>45771.905150462961</v>
       </c>
       <c r="B19" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -3538,7 +3541,7 @@
         <v>45776.095324074071</v>
       </c>
       <c r="B20" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C20">
         <v>18</v>
@@ -3555,7 +3558,7 @@
         <v>45772.951678240737</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -3572,7 +3575,7 @@
         <v>45772.998900462961</v>
       </c>
       <c r="B22" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -3589,7 +3592,7 @@
         <v>45774.632800925923</v>
       </c>
       <c r="B23" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -3606,7 +3609,7 @@
         <v>45774.623078703706</v>
       </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -3623,7 +3626,7 @@
         <v>45776.752511574072</v>
       </c>
       <c r="B25" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -3640,7 +3643,7 @@
         <v>45776.842094907406</v>
       </c>
       <c r="B26" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -3657,7 +3660,7 @@
         <v>45776.736539351848</v>
       </c>
       <c r="B27" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -3674,7 +3677,7 @@
         <v>45775.577800925923</v>
       </c>
       <c r="B28" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C28">
         <v>9</v>
@@ -3691,7 +3694,7 @@
         <v>45770.897002314814</v>
       </c>
       <c r="B29" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -3708,7 +3711,7 @@
         <v>45770.978252314817</v>
       </c>
       <c r="B30" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -3725,7 +3728,7 @@
         <v>45770.881030092591</v>
       </c>
       <c r="B31" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -3742,7 +3745,7 @@
         <v>45769.420787037037</v>
       </c>
       <c r="B32" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C32">
         <v>13</v>
@@ -3759,7 +3762,7 @@
         <v>45769.31523148148</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C33">
         <v>18</v>
@@ -3776,7 +3779,7 @@
         <v>45769.429814814815</v>
       </c>
       <c r="B34" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C34">
         <v>19</v>
@@ -3793,7 +3796,7 @@
         <v>45774.481516203705</v>
       </c>
       <c r="B35" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C35">
         <v>11</v>
@@ -3810,7 +3813,7 @@
         <v>45774.512071759258</v>
       </c>
       <c r="B36" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C36">
         <v>16</v>
@@ -3827,7 +3830,7 @@
         <v>45767.827662037038</v>
       </c>
       <c r="B37" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C37">
         <v>13</v>
@@ -3844,7 +3847,7 @@
         <v>45767.653009259258</v>
       </c>
       <c r="B38" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C38">
         <v>21</v>
@@ -3861,7 +3864,7 @@
         <v>45767.64675925926</v>
       </c>
       <c r="B39" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C39">
         <v>22</v>
@@ -3878,7 +3881,7 @@
         <v>45767.643287037034</v>
       </c>
       <c r="B40" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C40">
         <v>17</v>
@@ -3895,7 +3898,7 @@
         <v>45771.897499999999</v>
       </c>
       <c r="B41" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C41">
         <v>24</v>
@@ -3912,7 +3915,7 @@
         <v>45771.847500000003</v>
       </c>
       <c r="B42" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C42">
         <v>11</v>
@@ -3929,7 +3932,7 @@
         <v>45771.864861111113</v>
       </c>
       <c r="B43" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C43">
         <v>20</v>
@@ -3946,7 +3949,7 @@
         <v>45770.789895833332</v>
       </c>
       <c r="B44" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -3963,7 +3966,7 @@
         <v>45770.845451388886</v>
       </c>
       <c r="B45" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C45">
         <v>16</v>
@@ -3980,7 +3983,7 @@
         <v>45775.95484953704</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C46">
         <v>7</v>
@@ -3997,7 +4000,7 @@
         <v>45771.264999999999</v>
       </c>
       <c r="B47" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C47">
         <v>10</v>
@@ -4014,7 +4017,7 @@
         <v>45771.317083333335</v>
       </c>
       <c r="B48" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C48">
         <v>24</v>
@@ -4031,7 +4034,7 @@
         <v>45768.628807870373</v>
       </c>
       <c r="B49" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -4048,7 +4051,7 @@
         <v>45771.973067129627</v>
       </c>
       <c r="B50" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -4065,7 +4068,7 @@
         <v>45771.980011574073</v>
       </c>
       <c r="B51" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C51">
         <v>9</v>
@@ -4082,7 +4085,7 @@
         <v>45771.966817129629</v>
       </c>
       <c r="B52" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -4099,7 +4102,7 @@
         <v>45768.569814814815</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C53">
         <v>10</v>
@@ -4116,7 +4119,7 @@
         <v>45771.736701388887</v>
       </c>
       <c r="B54" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C54">
         <v>10</v>
@@ -4133,7 +4136,7 @@
         <v>45771.785312499997</v>
       </c>
       <c r="B55" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C55">
         <v>22</v>
@@ -4150,7 +4153,7 @@
         <v>45771.780451388891</v>
       </c>
       <c r="B56" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="C56">
         <v>24</v>
@@ -4167,7 +4170,7 @@
         <v>45772.420752314814</v>
       </c>
       <c r="B57" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C57">
         <v>25</v>
@@ -4184,7 +4187,7 @@
         <v>45772.464502314811</v>
       </c>
       <c r="B58" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C58">
         <v>22</v>
@@ -4201,7 +4204,7 @@
         <v>45772.375613425924</v>
       </c>
       <c r="B59" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C59">
         <v>16</v>
@@ -4218,7 +4221,7 @@
         <v>45767.599027777775</v>
       </c>
       <c r="B60" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C60">
         <v>14</v>
@@ -4235,7 +4238,7 @@
         <v>45774.196226851855</v>
       </c>
       <c r="B61" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -4252,7 +4255,7 @@
         <v>45774.178171296298</v>
       </c>
       <c r="B62" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C62">
         <v>18</v>
@@ -4269,7 +4272,7 @@
         <v>45774.240671296298</v>
       </c>
       <c r="B63" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -4301,10 +4304,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4567,30 +4570,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="E1" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B2">
         <v>2.2999999999999998</v>
       </c>
       <c r="C2" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="D2" s="2">
         <v>45768</v>
@@ -4601,13 +4604,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B3">
         <v>4.3</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="D3" s="2">
         <v>45769</v>
@@ -4618,13 +4621,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B4">
         <v>1.9</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="D4" s="2">
         <v>45772</v>
@@ -4635,13 +4638,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B5">
         <v>1.8</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="D5" s="2">
         <v>45772</v>
@@ -4652,13 +4655,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B6">
         <v>3.6</v>
       </c>
       <c r="C6" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="D6" s="2">
         <v>45772</v>
@@ -4669,13 +4672,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B7">
         <v>3.9</v>
       </c>
       <c r="C7" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="D7" s="2">
         <v>45774</v>
@@ -4686,13 +4689,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B8">
         <v>4.3</v>
       </c>
       <c r="C8" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="D8" s="2">
         <v>45770</v>
@@ -4703,13 +4706,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B9">
         <v>3.9</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="D9" s="2">
         <v>45768</v>
@@ -4720,13 +4723,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B10">
         <v>1.6</v>
       </c>
       <c r="C10" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="D10" s="2">
         <v>45768</v>
@@ -4737,13 +4740,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="D11" s="2">
         <v>45768</v>
@@ -4754,13 +4757,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B12">
         <v>4.9000000000000004</v>
       </c>
       <c r="C12" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
       <c r="D12" s="2">
         <v>45770</v>
@@ -4771,13 +4774,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="D13" s="2">
         <v>45770</v>
@@ -4788,13 +4791,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B14">
         <v>3.1</v>
       </c>
       <c r="C14" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
       <c r="D14" s="2">
         <v>45776</v>
@@ -4805,13 +4808,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B15">
         <v>2.2999999999999998</v>
       </c>
       <c r="C15" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="D15" s="2">
         <v>45776</v>
@@ -4822,13 +4825,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B16">
         <v>1.5</v>
       </c>
       <c r="C16" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="D16" s="2">
         <v>45776</v>
@@ -4839,13 +4842,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B17">
         <v>2.4</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="D17" s="2">
         <v>45771</v>
@@ -4856,13 +4859,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B18">
         <v>4.0999999999999996</v>
       </c>
       <c r="C18" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="D18" s="2">
         <v>45771</v>
@@ -4873,13 +4876,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B19">
         <v>4.2</v>
       </c>
       <c r="C19" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="D19" s="2">
         <v>45771</v>
@@ -4890,13 +4893,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B20">
         <v>4.4000000000000004</v>
       </c>
       <c r="C20" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="D20" s="2">
         <v>45776</v>
@@ -4907,13 +4910,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B21">
         <v>4.7</v>
       </c>
       <c r="C21" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
       <c r="D21" s="2">
         <v>45772</v>
@@ -4924,13 +4927,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B22">
         <v>4.8</v>
       </c>
       <c r="C22" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
       <c r="D22" s="2">
         <v>45772</v>
@@ -4941,13 +4944,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B23">
         <v>1.3</v>
       </c>
       <c r="C23" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
       <c r="D23" s="2">
         <v>45774</v>
@@ -4958,13 +4961,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B24">
         <v>2.2000000000000002</v>
       </c>
       <c r="C24" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
       <c r="D24" s="2">
         <v>45774</v>
@@ -4975,13 +4978,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>347</v>
+        <v>297</v>
       </c>
       <c r="D25" s="2">
         <v>45776</v>
@@ -4992,13 +4995,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B26">
         <v>1.1000000000000001</v>
       </c>
       <c r="C26" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="D26" s="2">
         <v>45776</v>
@@ -5009,13 +5012,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="D27" s="2">
         <v>45776</v>
@@ -5026,13 +5029,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B28">
         <v>2.4</v>
       </c>
       <c r="C28" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D28" s="2">
         <v>45775</v>
@@ -5043,13 +5046,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B29">
         <v>1.7</v>
       </c>
       <c r="C29" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
       <c r="D29" s="2">
         <v>45770</v>
@@ -5060,13 +5063,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B30">
         <v>4.5999999999999996</v>
       </c>
       <c r="C30" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="D30" s="2">
         <v>45770</v>
@@ -5077,13 +5080,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B31">
         <v>4.9000000000000004</v>
       </c>
       <c r="C31" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
       <c r="D31" s="2">
         <v>45770</v>
@@ -5094,13 +5097,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B32">
         <v>4.4000000000000004</v>
       </c>
       <c r="C32" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="D32" s="2">
         <v>45769</v>
@@ -5111,13 +5114,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B33">
         <v>4.5</v>
       </c>
       <c r="C33" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
       <c r="D33" s="2">
         <v>45769</v>
@@ -5128,13 +5131,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B34">
         <v>3.9</v>
       </c>
       <c r="C34" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="D34" s="2">
         <v>45769</v>
@@ -5145,13 +5148,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B35">
         <v>1.6</v>
       </c>
       <c r="C35" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
       <c r="D35" s="2">
         <v>45774</v>
@@ -5162,13 +5165,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B36">
         <v>1.8</v>
       </c>
       <c r="C36" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
       <c r="D36" s="2">
         <v>45774</v>
@@ -5179,13 +5182,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B37">
         <v>1.4</v>
       </c>
       <c r="C37" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="D37" s="2">
         <v>45767</v>
@@ -5196,13 +5199,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B38">
         <v>2.2999999999999998</v>
       </c>
       <c r="C38" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="D38" s="2">
         <v>45767</v>
@@ -5213,13 +5216,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B39">
         <v>3.1</v>
       </c>
       <c r="C39" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
       <c r="D39" s="2">
         <v>45767</v>
@@ -5230,13 +5233,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B40">
         <v>3.2</v>
       </c>
       <c r="C40" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="D40" s="2">
         <v>45767</v>
@@ -5247,13 +5250,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B41">
         <v>2.8</v>
       </c>
       <c r="C41" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
       <c r="D41" s="2">
         <v>45771</v>
@@ -5272,13 +5275,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C60B75A-1102-49C9-8546-841C09729105}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -5286,402 +5291,402 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>324</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>326</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>327</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>328</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>329</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>330</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>331</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>332</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>333</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>334</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>335</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>336</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>337</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>339</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>340</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>341</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>342</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>343</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>344</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>345</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>346</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>347</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>348</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>349</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>350</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>351</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>352</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>353</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>354</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>356</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>357</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>358</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>359</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>360</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>361</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>362</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>363</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>364</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>365</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -5693,7 +5698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A83C84A-2880-448C-B930-C4965EEB4C41}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -5701,16 +5706,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="C1" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6080,16 +6085,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6097,13 +6102,13 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6111,13 +6116,13 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6125,13 +6130,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6139,13 +6144,13 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -6153,13 +6158,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -6167,13 +6172,13 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -6181,13 +6186,13 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -6195,13 +6200,13 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -6209,13 +6214,13 @@
         <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -6223,13 +6228,13 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -6249,10 +6254,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6928,13 +6933,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -7397,39 +7402,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="G1" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C2">
         <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E2">
         <v>19</v>
@@ -7438,24 +7443,24 @@
         <v>3.69</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -7464,24 +7469,24 @@
         <v>10.65</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C4">
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -7490,24 +7495,24 @@
         <v>8.01</v>
       </c>
       <c r="G4" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C5">
         <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -7516,24 +7521,24 @@
         <v>13.32</v>
       </c>
       <c r="G5" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E6">
         <v>11</v>
@@ -7542,24 +7547,24 @@
         <v>14.98</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H6" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C7">
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E7">
         <v>13</v>
@@ -7568,24 +7573,24 @@
         <v>13.95</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H7" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C8">
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -7594,24 +7599,24 @@
         <v>3.21</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C9">
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -7620,24 +7625,24 @@
         <v>10.33</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H9" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C10">
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -7646,24 +7651,24 @@
         <v>10.62</v>
       </c>
       <c r="G10" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C11">
         <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E11">
         <v>16</v>
@@ -7672,24 +7677,24 @@
         <v>6.04</v>
       </c>
       <c r="G11" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H11" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C12">
         <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="E12">
         <v>20</v>
@@ -7698,24 +7703,24 @@
         <v>5.09</v>
       </c>
       <c r="G12" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H12" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C13">
         <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="E13">
         <v>17</v>
@@ -7724,24 +7729,24 @@
         <v>13.49</v>
       </c>
       <c r="G13" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H13" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C14">
         <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E14">
         <v>16</v>
@@ -7750,24 +7755,24 @@
         <v>6.78</v>
       </c>
       <c r="G14" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H14" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C15">
         <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -7776,24 +7781,24 @@
         <v>13.75</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H15" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C16">
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E16">
         <v>8</v>
@@ -7802,24 +7807,24 @@
         <v>6.3</v>
       </c>
       <c r="G16" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C17">
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E17">
         <v>19</v>
@@ -7828,24 +7833,24 @@
         <v>13.25</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H17" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C18">
         <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -7854,24 +7859,24 @@
         <v>3.61</v>
       </c>
       <c r="G18" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H18" t="s">
-        <v>220</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C19">
         <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -7880,24 +7885,24 @@
         <v>5.15</v>
       </c>
       <c r="G19" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="H19" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C20">
         <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E20">
         <v>13</v>
@@ -7906,24 +7911,24 @@
         <v>9.85</v>
       </c>
       <c r="G20" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H20" t="s">
-        <v>224</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -7932,24 +7937,24 @@
         <v>3.71</v>
       </c>
       <c r="G21" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>226</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C22">
         <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="E22">
         <v>11</v>
@@ -7958,24 +7963,24 @@
         <v>14.57</v>
       </c>
       <c r="G22" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>228</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C23">
         <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="E23">
         <v>11</v>
@@ -7984,24 +7989,24 @@
         <v>6.82</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H23" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>181</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C24">
         <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E24">
         <v>16</v>
@@ -8010,24 +8015,24 @@
         <v>13.97</v>
       </c>
       <c r="G24" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>232</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C25">
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E25">
         <v>19</v>
@@ -8036,24 +8041,24 @@
         <v>6.89</v>
       </c>
       <c r="G25" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C26">
         <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E26">
         <v>7</v>
@@ -8062,10 +8067,10 @@
         <v>4.76</v>
       </c>
       <c r="G26" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H26" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -8085,22 +8090,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -8108,13 +8113,13 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>397369864</v>
@@ -8128,16 +8133,16 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>194</v>
       </c>
       <c r="F3">
         <v>18</v>
@@ -8148,16 +8153,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="F4">
         <v>16</v>
@@ -8168,16 +8173,16 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="E5" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="F5">
         <v>14</v>
@@ -8188,13 +8193,13 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <v>675258537</v>
@@ -8208,16 +8213,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="E7" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -8228,16 +8233,16 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="F8">
         <v>8</v>
@@ -8248,13 +8253,13 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="E9">
         <v>307850319</v>
@@ -8268,13 +8273,13 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>219</v>
       </c>
       <c r="E10">
         <v>472792509</v>
@@ -8288,16 +8293,16 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="D11" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="E11" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -8308,16 +8313,16 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>226</v>
       </c>
       <c r="E12" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="F12">
         <v>9</v>
@@ -8328,16 +8333,16 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="C13" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="F13">
         <v>23</v>
@@ -8348,16 +8353,16 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>284</v>
+        <v>234</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -8368,16 +8373,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="C15" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="E15" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="F15">
         <v>25</v>
@@ -8388,16 +8393,16 @@
         <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="C16" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
       <c r="D16" t="s">
-        <v>291</v>
+        <v>241</v>
       </c>
       <c r="E16" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="F16">
         <v>5</v>
@@ -8408,16 +8413,16 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>293</v>
+        <v>243</v>
       </c>
       <c r="D17" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
       <c r="E17" t="s">
-        <v>295</v>
+        <v>245</v>
       </c>
       <c r="F17">
         <v>15</v>
@@ -8428,13 +8433,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>296</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="D18" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="E18">
         <v>587770947</v>
@@ -8448,13 +8453,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>299</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D19" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="E19">
         <v>805925841</v>
@@ -8468,16 +8473,16 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="C20" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="D20" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="E20" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="F20">
         <v>24</v>
@@ -8488,16 +8493,16 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>305</v>
+        <v>255</v>
       </c>
       <c r="C21" t="s">
-        <v>306</v>
+        <v>256</v>
       </c>
       <c r="D21" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="E21" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
       <c r="F21">
         <v>1</v>

</xml_diff>